<commit_message>
Part 2 excel completed
</commit_message>
<xml_diff>
--- a/Assignment 4/Elctrical_assignment_Answers_template.xlsx
+++ b/Assignment 4/Elctrical_assignment_Answers_template.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="5" rupBuild="28025"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="5" rupBuild="29231"/>
   <workbookPr showInkAnnotation="0" autoCompressPictures="0"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://scaleore-my.sharepoint.com/personal/bart_scaleoffshore_com/Documents/02 tu Delft/ORT/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://d.docs.live.net/5e081d09bad3eec4/Documents/TU Delft/Y2/Q1/Offshore Renewables/Offshore-Renewable-Technologies/Assignment 4/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="4" documentId="8_{BB568C5D-74B7-471F-A9F9-106ECE79A48D}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{23B7C1F2-2880-4FBF-8B6C-C99F1E66CE25}"/>
+  <xr:revisionPtr revIDLastSave="75" documentId="8_{BB568C5D-74B7-471F-A9F9-106ECE79A48D}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{8D44AC10-BE69-430B-A3D4-EC9BA4BB729E}"/>
   <bookViews>
-    <workbookView xWindow="-103" yWindow="-103" windowWidth="21600" windowHeight="13749" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-98" yWindow="-98" windowWidth="21795" windowHeight="13695" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="WTG Yield Wake" sheetId="1" r:id="rId1"/>
@@ -251,10 +251,10 @@
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
   <numFmts count="4">
-    <numFmt numFmtId="43" formatCode="_ * #,##0.00_ ;_ * \-#,##0.00_ ;_ * &quot;-&quot;??_ ;_ @_ "/>
-    <numFmt numFmtId="164" formatCode="0.000"/>
-    <numFmt numFmtId="165" formatCode="_ * #,##0_ ;_ * \-#,##0_ ;_ * &quot;-&quot;??_ ;_ @_ "/>
-    <numFmt numFmtId="166" formatCode="0.0"/>
+    <numFmt numFmtId="164" formatCode="_ * #,##0.00_ ;_ * \-#,##0.00_ ;_ * &quot;-&quot;??_ ;_ @_ "/>
+    <numFmt numFmtId="165" formatCode="0.000"/>
+    <numFmt numFmtId="166" formatCode="_ * #,##0_ ;_ * \-#,##0_ ;_ * &quot;-&quot;??_ ;_ @_ "/>
+    <numFmt numFmtId="167" formatCode="0.0"/>
   </numFmts>
   <fonts count="9" x14ac:knownFonts="1">
     <font>
@@ -793,9 +793,9 @@
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="43" fontId="4" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="164" fontId="4" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="125">
+  <cellXfs count="122">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="6" fillId="0" borderId="0" xfId="0" applyFont="1"/>
@@ -816,8 +816,8 @@
     <xf numFmtId="1" fontId="7" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1">
       <alignment horizontal="right"/>
     </xf>
-    <xf numFmtId="165" fontId="6" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
-    <xf numFmtId="165" fontId="6" fillId="2" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyAlignment="1">
+    <xf numFmtId="166" fontId="6" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
+    <xf numFmtId="166" fontId="6" fillId="2" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="right"/>
     </xf>
     <xf numFmtId="0" fontId="6" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
@@ -862,7 +862,7 @@
     <xf numFmtId="0" fontId="7" fillId="2" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="165" fontId="7" fillId="2" borderId="4" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="166" fontId="7" fillId="2" borderId="4" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
@@ -893,51 +893,45 @@
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="7" fillId="2" borderId="11" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="164" fontId="7" fillId="2" borderId="4" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="164" fontId="7" fillId="2" borderId="8" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="164" fontId="7" fillId="2" borderId="11" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="164" fontId="7" fillId="2" borderId="6" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="164" fontId="7" fillId="2" borderId="9" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="164" fontId="7" fillId="2" borderId="12" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="43" fontId="7" fillId="2" borderId="4" xfId="42" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="165" fontId="7" fillId="2" borderId="4" xfId="42" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="165" fontId="7" fillId="2" borderId="8" xfId="42" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="165" fontId="7" fillId="2" borderId="4" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="165" fontId="7" fillId="2" borderId="8" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="165" fontId="7" fillId="2" borderId="11" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="165" fontId="7" fillId="2" borderId="6" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="165" fontId="7" fillId="2" borderId="9" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="165" fontId="7" fillId="2" borderId="12" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="164" fontId="7" fillId="2" borderId="4" xfId="42" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="166" fontId="7" fillId="2" borderId="4" xfId="42" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="166" fontId="7" fillId="2" borderId="8" xfId="42" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="9" fontId="0" fillId="2" borderId="8" xfId="21" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="43" fontId="7" fillId="2" borderId="6" xfId="42" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="165" fontId="7" fillId="2" borderId="6" xfId="42" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="164" fontId="7" fillId="2" borderId="6" xfId="42" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="166" fontId="7" fillId="2" borderId="6" xfId="42" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="9" fontId="0" fillId="2" borderId="9" xfId="21" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="6" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="right"/>
     </xf>
-    <xf numFmtId="166" fontId="7" fillId="2" borderId="14" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="167" fontId="7" fillId="2" borderId="14" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="43" fontId="7" fillId="2" borderId="14" xfId="42" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="166" fontId="7" fillId="2" borderId="14" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="166" fontId="7" fillId="2" borderId="20" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="164" fontId="7" fillId="2" borderId="14" xfId="42" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="167" fontId="7" fillId="2" borderId="14" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="167" fontId="7" fillId="2" borderId="20" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="7" fillId="2" borderId="21" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="166" fontId="7" fillId="2" borderId="21" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="167" fontId="7" fillId="2" borderId="21" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="6" fillId="2" borderId="10" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="166" fontId="7" fillId="4" borderId="11" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="166" fontId="7" fillId="4" borderId="12" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="167" fontId="7" fillId="4" borderId="11" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="167" fontId="7" fillId="4" borderId="12" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="7" fillId="2" borderId="23" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="1" fontId="7" fillId="4" borderId="7" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="164" fontId="7" fillId="4" borderId="24" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="164" fontId="7" fillId="4" borderId="25" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="165" fontId="7" fillId="4" borderId="24" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="6" fillId="2" borderId="22" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
@@ -953,29 +947,11 @@
     <xf numFmtId="0" fontId="6" fillId="2" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="166" fontId="7" fillId="2" borderId="27" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="167" fontId="7" fillId="2" borderId="27" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="166" fontId="7" fillId="2" borderId="20" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="167" fontId="7" fillId="2" borderId="20" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="2" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="2" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="2" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="2" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="2" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left"/>
     </xf>
     <xf numFmtId="0" fontId="7" fillId="3" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
     <xf numFmtId="0" fontId="7" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
@@ -983,7 +959,7 @@
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="1" fontId="6" fillId="2" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1"/>
-    <xf numFmtId="165" fontId="6" fillId="2" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyAlignment="1">
+    <xf numFmtId="166" fontId="6" fillId="2" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="8" fillId="0" borderId="0" xfId="0" applyFont="1"/>
@@ -1007,10 +983,9 @@
     <xf numFmtId="1" fontId="7" fillId="4" borderId="28" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="164" fontId="7" fillId="4" borderId="29" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="165" fontId="7" fillId="4" borderId="29" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="7" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="6" fillId="2" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
@@ -1061,7 +1036,7 @@
     <xf numFmtId="0" fontId="6" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="166" fontId="7" fillId="2" borderId="13" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="167" fontId="7" fillId="2" borderId="13" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="6" fillId="2" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
@@ -1072,6 +1047,24 @@
     </xf>
     <xf numFmtId="0" fontId="7" fillId="2" borderId="31" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="2" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="2" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="2" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="2" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="2" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left"/>
     </xf>
   </cellXfs>
   <cellStyles count="43">
@@ -1117,7 +1110,7 @@
     <cellStyle name="Hyperlink" xfId="38" builtinId="8" hidden="1"/>
     <cellStyle name="Hyperlink" xfId="40" builtinId="8" hidden="1"/>
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
-    <cellStyle name="Percent" xfId="21" builtinId="5"/>
+    <cellStyle name="Per cent" xfId="21" builtinId="5"/>
   </cellStyles>
   <dxfs count="0"/>
   <tableStyles count="0" defaultTableStyle="TableStyleMedium9" defaultPivotStyle="PivotStyleMedium4"/>
@@ -1203,7 +1196,7 @@
 <file path=xl/charts/chart1.xml><?xml version="1.0" encoding="utf-8"?>
 <c:chartSpace xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:c16r2="http://schemas.microsoft.com/office/drawing/2015/06/chart">
   <c:date1904 val="0"/>
-  <c:lang val="en-US"/>
+  <c:lang val="en-GB"/>
   <c:roundedCorners val="0"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice xmlns:c14="http://schemas.microsoft.com/office/drawing/2007/8/2/chart" Requires="c14">
@@ -1631,7 +1624,7 @@
 <file path=xl/charts/chart2.xml><?xml version="1.0" encoding="utf-8"?>
 <c:chartSpace xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:c16r2="http://schemas.microsoft.com/office/drawing/2015/06/chart">
   <c:date1904 val="0"/>
-  <c:lang val="en-US"/>
+  <c:lang val="en-GB"/>
   <c:roundedCorners val="0"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice xmlns:c14="http://schemas.microsoft.com/office/drawing/2007/8/2/chart" Requires="c14">
@@ -2039,7 +2032,7 @@
 <file path=xl/charts/chart3.xml><?xml version="1.0" encoding="utf-8"?>
 <c:chartSpace xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:c16r2="http://schemas.microsoft.com/office/drawing/2015/06/chart">
   <c:date1904 val="0"/>
-  <c:lang val="en-US"/>
+  <c:lang val="en-GB"/>
   <c:roundedCorners val="0"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice xmlns:c14="http://schemas.microsoft.com/office/drawing/2007/8/2/chart" Requires="c14">
@@ -2459,7 +2452,7 @@
 <file path=xl/charts/chart4.xml><?xml version="1.0" encoding="utf-8"?>
 <c:chartSpace xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:c16r2="http://schemas.microsoft.com/office/drawing/2015/06/chart">
   <c:date1904 val="0"/>
-  <c:lang val="en-US"/>
+  <c:lang val="en-GB"/>
   <c:roundedCorners val="0"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice xmlns:c14="http://schemas.microsoft.com/office/drawing/2007/8/2/chart" Requires="c14">
@@ -3008,6 +3001,7 @@
     </c:plotArea>
     <c:plotVisOnly val="1"/>
     <c:dispBlanksAs val="gap"/>
+    <c:showDLblsOverMax val="0"/>
     <c:extLst>
       <c:ext xmlns:c16r3="http://schemas.microsoft.com/office/drawing/2017/03/chart" uri="{56B9EC1D-385E-4148-901F-78D8002777C0}">
         <c16r3:dataDisplayOptions16>
@@ -3015,7 +3009,6 @@
         </c16r3:dataDisplayOptions16>
       </c:ext>
     </c:extLst>
-    <c:showDLblsOverMax val="0"/>
   </c:chart>
   <c:spPr>
     <a:solidFill>
@@ -4090,37 +4083,37 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="B2:M46"/>
   <sheetViews>
-    <sheetView zoomScale="70" zoomScaleNormal="70" workbookViewId="0">
-      <selection activeCell="W19" sqref="W19"/>
+    <sheetView topLeftCell="C29" zoomScale="155" zoomScaleNormal="70" workbookViewId="0">
+      <selection activeCell="J43" sqref="J43"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="8.84375" defaultRowHeight="12.9" x14ac:dyDescent="0.35"/>
+  <sheetFormatPr defaultColWidth="8.86328125" defaultRowHeight="13.15" x14ac:dyDescent="0.4"/>
   <cols>
-    <col min="1" max="1" width="8.84375" style="9"/>
-    <col min="2" max="2" width="11.3828125" style="9" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="15.15234375" style="9" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="8.86328125" style="9"/>
+    <col min="2" max="2" width="11.3984375" style="9" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="15.1328125" style="9" bestFit="1" customWidth="1"/>
     <col min="4" max="4" width="10" style="9" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="6.53515625" style="9" bestFit="1" customWidth="1"/>
-    <col min="6" max="6" width="5.84375" style="9" bestFit="1" customWidth="1"/>
-    <col min="7" max="7" width="11.53515625" style="9" customWidth="1"/>
-    <col min="8" max="8" width="13.3828125" style="9" bestFit="1" customWidth="1"/>
-    <col min="9" max="9" width="14.3828125" style="9" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="6.53125" style="9" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="5.86328125" style="9" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="11.53125" style="9" customWidth="1"/>
+    <col min="8" max="8" width="13.3984375" style="9" bestFit="1" customWidth="1"/>
+    <col min="9" max="9" width="14.3984375" style="9" bestFit="1" customWidth="1"/>
     <col min="10" max="10" width="10" style="9" bestFit="1" customWidth="1"/>
-    <col min="11" max="11" width="12.53515625" style="9" customWidth="1"/>
-    <col min="12" max="12" width="13.84375" style="9" bestFit="1" customWidth="1"/>
-    <col min="13" max="16384" width="8.84375" style="9"/>
+    <col min="11" max="11" width="12.53125" style="9" customWidth="1"/>
+    <col min="12" max="12" width="13.86328125" style="9" bestFit="1" customWidth="1"/>
+    <col min="13" max="16384" width="8.86328125" style="9"/>
   </cols>
   <sheetData>
-    <row r="2" spans="2:12" ht="13.3" thickBot="1" x14ac:dyDescent="0.4">
+    <row r="2" spans="2:12" ht="13.5" thickBot="1" x14ac:dyDescent="0.45">
       <c r="B2" s="2" t="s">
         <v>11</v>
       </c>
     </row>
-    <row r="3" spans="2:12" x14ac:dyDescent="0.35">
-      <c r="B3" s="79" t="s">
+    <row r="3" spans="2:12" x14ac:dyDescent="0.4">
+      <c r="B3" s="118" t="s">
         <v>3</v>
       </c>
-      <c r="C3" s="80"/>
+      <c r="C3" s="119"/>
       <c r="D3" s="34">
         <v>280</v>
       </c>
@@ -4128,11 +4121,11 @@
         <v>6</v>
       </c>
     </row>
-    <row r="4" spans="2:12" x14ac:dyDescent="0.35">
-      <c r="B4" s="77" t="s">
+    <row r="4" spans="2:12" x14ac:dyDescent="0.4">
+      <c r="B4" s="116" t="s">
         <v>4</v>
       </c>
-      <c r="C4" s="78"/>
+      <c r="C4" s="117"/>
       <c r="D4" s="35">
         <f>PI()*D3^2*(1/4)</f>
         <v>61575.216010359945</v>
@@ -4141,11 +4134,11 @@
         <v>7</v>
       </c>
     </row>
-    <row r="5" spans="2:12" x14ac:dyDescent="0.35">
-      <c r="B5" s="77" t="s">
+    <row r="5" spans="2:12" x14ac:dyDescent="0.4">
+      <c r="B5" s="116" t="s">
         <v>54</v>
       </c>
-      <c r="C5" s="78"/>
+      <c r="C5" s="117"/>
       <c r="D5" s="36">
         <v>20</v>
       </c>
@@ -4153,11 +4146,11 @@
         <v>43</v>
       </c>
     </row>
-    <row r="6" spans="2:12" x14ac:dyDescent="0.35">
-      <c r="B6" s="77" t="s">
+    <row r="6" spans="2:12" x14ac:dyDescent="0.4">
+      <c r="B6" s="116" t="s">
         <v>18</v>
       </c>
-      <c r="C6" s="78"/>
+      <c r="C6" s="117"/>
       <c r="D6" s="35">
         <f>D5*1000000/D4</f>
         <v>324.80600630999049</v>
@@ -4166,11 +4159,11 @@
         <v>19</v>
       </c>
     </row>
-    <row r="7" spans="2:12" x14ac:dyDescent="0.35">
-      <c r="B7" s="77" t="s">
+    <row r="7" spans="2:12" x14ac:dyDescent="0.4">
+      <c r="B7" s="116" t="s">
         <v>52</v>
       </c>
-      <c r="C7" s="78"/>
+      <c r="C7" s="117"/>
       <c r="D7" s="36">
         <v>7</v>
       </c>
@@ -4178,11 +4171,11 @@
         <v>8</v>
       </c>
     </row>
-    <row r="8" spans="2:12" x14ac:dyDescent="0.35">
-      <c r="B8" s="77" t="s">
+    <row r="8" spans="2:12" x14ac:dyDescent="0.4">
+      <c r="B8" s="116" t="s">
         <v>53</v>
       </c>
-      <c r="C8" s="78"/>
+      <c r="C8" s="117"/>
       <c r="D8" s="35">
         <f>PI()*D3*D7/60</f>
         <v>102.62536001726657</v>
@@ -4192,11 +4185,11 @@
       </c>
       <c r="F8" s="10"/>
     </row>
-    <row r="9" spans="2:12" ht="13.3" thickBot="1" x14ac:dyDescent="0.4">
-      <c r="B9" s="81" t="s">
+    <row r="9" spans="2:12" ht="13.5" thickBot="1" x14ac:dyDescent="0.45">
+      <c r="B9" s="120" t="s">
         <v>5</v>
       </c>
-      <c r="C9" s="82"/>
+      <c r="C9" s="121"/>
       <c r="D9" s="37">
         <v>160</v>
       </c>
@@ -4204,7 +4197,7 @@
         <v>6</v>
       </c>
     </row>
-    <row r="10" spans="2:12" x14ac:dyDescent="0.35">
+    <row r="10" spans="2:12" x14ac:dyDescent="0.4">
       <c r="B10" s="12"/>
       <c r="C10" s="12"/>
       <c r="D10" s="13"/>
@@ -4212,7 +4205,7 @@
         <v>42</v>
       </c>
     </row>
-    <row r="11" spans="2:12" ht="13.3" thickBot="1" x14ac:dyDescent="0.4">
+    <row r="11" spans="2:12" ht="13.5" thickBot="1" x14ac:dyDescent="0.45">
       <c r="B11" s="2" t="s">
         <v>56</v>
       </c>
@@ -4223,7 +4216,7 @@
         <v>80</v>
       </c>
     </row>
-    <row r="12" spans="2:12" ht="25.75" x14ac:dyDescent="0.35">
+    <row r="12" spans="2:12" ht="26.25" x14ac:dyDescent="0.4">
       <c r="B12" s="38" t="s">
         <v>58</v>
       </c>
@@ -4240,7 +4233,7 @@
         <v>21</v>
       </c>
       <c r="G12" s="18"/>
-      <c r="H12" s="89" t="s">
+      <c r="H12" s="81" t="s">
         <v>59</v>
       </c>
       <c r="I12" s="39" t="s">
@@ -4256,7 +4249,7 @@
         <v>33</v>
       </c>
     </row>
-    <row r="13" spans="2:12" x14ac:dyDescent="0.35">
+    <row r="13" spans="2:12" x14ac:dyDescent="0.4">
       <c r="B13" s="20" t="s">
         <v>1</v>
       </c>
@@ -4284,7 +4277,7 @@
         <v>26</v>
       </c>
     </row>
-    <row r="14" spans="2:12" x14ac:dyDescent="0.35">
+    <row r="14" spans="2:12" x14ac:dyDescent="0.4">
       <c r="B14" s="20">
         <f>H14</f>
         <v>0.5</v>
@@ -4316,7 +4309,7 @@
       <c r="K14" s="51"/>
       <c r="L14" s="11"/>
     </row>
-    <row r="15" spans="2:12" x14ac:dyDescent="0.35">
+    <row r="15" spans="2:12" x14ac:dyDescent="0.4">
       <c r="B15" s="20">
         <f t="shared" ref="B15:B41" si="0">H15</f>
         <v>1.5</v>
@@ -4348,7 +4341,7 @@
       <c r="K15" s="51"/>
       <c r="L15" s="11"/>
     </row>
-    <row r="16" spans="2:12" x14ac:dyDescent="0.35">
+    <row r="16" spans="2:12" x14ac:dyDescent="0.4">
       <c r="B16" s="20">
         <f t="shared" si="0"/>
         <v>2.5</v>
@@ -4380,7 +4373,7 @@
       <c r="K16" s="51"/>
       <c r="L16" s="11"/>
     </row>
-    <row r="17" spans="2:12" x14ac:dyDescent="0.35">
+    <row r="17" spans="2:12" x14ac:dyDescent="0.4">
       <c r="B17" s="20">
         <f t="shared" si="0"/>
         <v>3.5</v>
@@ -4417,7 +4410,7 @@
         <v>7246.5249857361696</v>
       </c>
     </row>
-    <row r="18" spans="2:12" x14ac:dyDescent="0.35">
+    <row r="18" spans="2:12" x14ac:dyDescent="0.4">
       <c r="B18" s="20">
         <f t="shared" si="0"/>
         <v>4.5</v>
@@ -4454,7 +4447,7 @@
         <v>36132.969087428872</v>
       </c>
     </row>
-    <row r="19" spans="2:12" x14ac:dyDescent="0.35">
+    <row r="19" spans="2:12" x14ac:dyDescent="0.4">
       <c r="B19" s="20">
         <f t="shared" si="0"/>
         <v>5.5</v>
@@ -4491,7 +4484,7 @@
         <v>93659.227887075074</v>
       </c>
     </row>
-    <row r="20" spans="2:12" x14ac:dyDescent="0.35">
+    <row r="20" spans="2:12" x14ac:dyDescent="0.4">
       <c r="B20" s="20">
         <f t="shared" si="0"/>
         <v>6.5</v>
@@ -4528,7 +4521,7 @@
         <v>186041.20624289944</v>
       </c>
     </row>
-    <row r="21" spans="2:12" x14ac:dyDescent="0.35">
+    <row r="21" spans="2:12" x14ac:dyDescent="0.4">
       <c r="B21" s="20">
         <f t="shared" si="0"/>
         <v>7.5</v>
@@ -4565,7 +4558,7 @@
         <v>319182.8734163898</v>
       </c>
     </row>
-    <row r="22" spans="2:12" x14ac:dyDescent="0.35">
+    <row r="22" spans="2:12" x14ac:dyDescent="0.4">
       <c r="B22" s="20">
         <f t="shared" si="0"/>
         <v>8.5</v>
@@ -4602,7 +4595,7 @@
         <v>488953.4761470104</v>
       </c>
     </row>
-    <row r="23" spans="2:12" x14ac:dyDescent="0.35">
+    <row r="23" spans="2:12" x14ac:dyDescent="0.4">
       <c r="B23" s="20">
         <f t="shared" si="0"/>
         <v>9.5</v>
@@ -4639,7 +4632,7 @@
         <v>653553.43702042813</v>
       </c>
     </row>
-    <row r="24" spans="2:12" x14ac:dyDescent="0.35">
+    <row r="24" spans="2:12" x14ac:dyDescent="0.4">
       <c r="B24" s="20">
         <f t="shared" si="0"/>
         <v>10.5</v>
@@ -4676,7 +4669,7 @@
         <v>770256.41341890593</v>
       </c>
     </row>
-    <row r="25" spans="2:12" x14ac:dyDescent="0.35">
+    <row r="25" spans="2:12" x14ac:dyDescent="0.4">
       <c r="B25" s="20">
         <f t="shared" si="0"/>
         <v>11.5</v>
@@ -4713,7 +4706,7 @@
         <v>808849.16043602966</v>
       </c>
     </row>
-    <row r="26" spans="2:12" x14ac:dyDescent="0.35">
+    <row r="26" spans="2:12" x14ac:dyDescent="0.4">
       <c r="B26" s="20">
         <f t="shared" si="0"/>
         <v>12.5</v>
@@ -4750,7 +4743,7 @@
         <v>746939.73612787831</v>
       </c>
     </row>
-    <row r="27" spans="2:12" x14ac:dyDescent="0.35">
+    <row r="27" spans="2:12" x14ac:dyDescent="0.4">
       <c r="B27" s="20">
         <f t="shared" si="0"/>
         <v>13.5</v>
@@ -4787,7 +4780,7 @@
         <v>617663.67086750141</v>
       </c>
     </row>
-    <row r="28" spans="2:12" x14ac:dyDescent="0.35">
+    <row r="28" spans="2:12" x14ac:dyDescent="0.4">
       <c r="B28" s="20">
         <f t="shared" si="0"/>
         <v>14.5</v>
@@ -4824,7 +4817,7 @@
         <v>469192.01473053574</v>
       </c>
     </row>
-    <row r="29" spans="2:12" x14ac:dyDescent="0.35">
+    <row r="29" spans="2:12" x14ac:dyDescent="0.4">
       <c r="B29" s="20">
         <f t="shared" si="0"/>
         <v>15.5</v>
@@ -4861,7 +4854,7 @@
         <v>338385.11752361641</v>
       </c>
     </row>
-    <row r="30" spans="2:12" x14ac:dyDescent="0.35">
+    <row r="30" spans="2:12" x14ac:dyDescent="0.4">
       <c r="B30" s="20">
         <f t="shared" si="0"/>
         <v>16.5</v>
@@ -4898,7 +4891,7 @@
         <v>252457.16514500129</v>
       </c>
     </row>
-    <row r="31" spans="2:12" x14ac:dyDescent="0.35">
+    <row r="31" spans="2:12" x14ac:dyDescent="0.4">
       <c r="B31" s="20">
         <f t="shared" si="0"/>
         <v>17.5</v>
@@ -4935,7 +4928,7 @@
         <v>198349.18860642804</v>
       </c>
     </row>
-    <row r="32" spans="2:12" x14ac:dyDescent="0.35">
+    <row r="32" spans="2:12" x14ac:dyDescent="0.4">
       <c r="B32" s="20">
         <f t="shared" si="0"/>
         <v>18.5</v>
@@ -4972,7 +4965,7 @@
         <v>160641.81635545334</v>
       </c>
     </row>
-    <row r="33" spans="2:13" x14ac:dyDescent="0.35">
+    <row r="33" spans="2:13" x14ac:dyDescent="0.4">
       <c r="B33" s="20">
         <f t="shared" si="0"/>
         <v>19.5</v>
@@ -5009,7 +5002,7 @@
         <v>121112.15473918998</v>
       </c>
     </row>
-    <row r="34" spans="2:13" x14ac:dyDescent="0.35">
+    <row r="34" spans="2:13" x14ac:dyDescent="0.4">
       <c r="B34" s="20">
         <f t="shared" si="0"/>
         <v>20.5</v>
@@ -5046,7 +5039,7 @@
         <v>85787.776273592885</v>
       </c>
     </row>
-    <row r="35" spans="2:13" x14ac:dyDescent="0.35">
+    <row r="35" spans="2:13" x14ac:dyDescent="0.4">
       <c r="B35" s="20">
         <f t="shared" si="0"/>
         <v>21.5</v>
@@ -5083,7 +5076,7 @@
         <v>60976.605684661612</v>
       </c>
     </row>
-    <row r="36" spans="2:13" x14ac:dyDescent="0.35">
+    <row r="36" spans="2:13" x14ac:dyDescent="0.4">
       <c r="B36" s="20">
         <f t="shared" si="0"/>
         <v>22.5</v>
@@ -5120,7 +5113,7 @@
         <v>41211.774876529918</v>
       </c>
     </row>
-    <row r="37" spans="2:13" x14ac:dyDescent="0.35">
+    <row r="37" spans="2:13" x14ac:dyDescent="0.4">
       <c r="B37" s="20">
         <f t="shared" si="0"/>
         <v>23.5</v>
@@ -5157,7 +5150,7 @@
         <v>24289.646284800005</v>
       </c>
     </row>
-    <row r="38" spans="2:13" x14ac:dyDescent="0.35">
+    <row r="38" spans="2:13" x14ac:dyDescent="0.4">
       <c r="B38" s="20">
         <f t="shared" si="0"/>
         <v>24.5</v>
@@ -5194,7 +5187,7 @@
         <v>12083.5593216</v>
       </c>
     </row>
-    <row r="39" spans="2:13" x14ac:dyDescent="0.35">
+    <row r="39" spans="2:13" x14ac:dyDescent="0.4">
       <c r="B39" s="20">
         <f t="shared" si="0"/>
         <v>25.5</v>
@@ -5231,7 +5224,7 @@
         <v>6213.9018239999987</v>
       </c>
     </row>
-    <row r="40" spans="2:13" x14ac:dyDescent="0.35">
+    <row r="40" spans="2:13" x14ac:dyDescent="0.4">
       <c r="B40" s="20">
         <f t="shared" si="0"/>
         <v>26.5</v>
@@ -5268,7 +5261,7 @@
         <v>2503.0646783999996</v>
       </c>
     </row>
-    <row r="41" spans="2:13" x14ac:dyDescent="0.35">
+    <row r="41" spans="2:13" x14ac:dyDescent="0.4">
       <c r="B41" s="20">
         <f t="shared" si="0"/>
         <v>27.5</v>
@@ -5305,7 +5298,7 @@
         <v>1102.7487744</v>
       </c>
     </row>
-    <row r="42" spans="2:13" ht="13.3" thickBot="1" x14ac:dyDescent="0.4">
+    <row r="42" spans="2:13" ht="13.5" thickBot="1" x14ac:dyDescent="0.45">
       <c r="B42" s="25">
         <f>H42</f>
         <v>28.5</v>
@@ -5341,8 +5334,8 @@
         <v>0</v>
       </c>
     </row>
-    <row r="43" spans="2:13" x14ac:dyDescent="0.35">
-      <c r="B43" s="88" t="s">
+    <row r="43" spans="2:13" x14ac:dyDescent="0.4">
+      <c r="B43" s="80" t="s">
         <v>57</v>
       </c>
       <c r="C43" s="12"/>
@@ -5359,7 +5352,7 @@
         <v>28</v>
       </c>
     </row>
-    <row r="45" spans="2:13" ht="13.3" thickBot="1" x14ac:dyDescent="0.4">
+    <row r="45" spans="2:13" ht="13.5" thickBot="1" x14ac:dyDescent="0.45">
       <c r="J45" s="16" t="s">
         <v>30</v>
       </c>
@@ -5370,7 +5363,7 @@
         <v>32</v>
       </c>
     </row>
-    <row r="46" spans="2:13" ht="13.3" thickBot="1" x14ac:dyDescent="0.4">
+    <row r="46" spans="2:13" ht="13.5" thickBot="1" x14ac:dyDescent="0.45">
       <c r="I46" s="2" t="s">
         <v>29</v>
       </c>
@@ -5409,23 +5402,23 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0100-000000000000}">
   <dimension ref="A1:O51"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A6" zoomScale="85" zoomScaleNormal="85" zoomScalePageLayoutView="125" workbookViewId="0">
-      <selection activeCell="U15" sqref="U15"/>
+    <sheetView tabSelected="1" topLeftCell="A15" zoomScaleNormal="100" zoomScalePageLayoutView="125" workbookViewId="0">
+      <selection activeCell="J33" sqref="J33"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="8.84375" defaultRowHeight="12.45" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr defaultColWidth="8.86328125" defaultRowHeight="12.75" x14ac:dyDescent="0.35"/>
   <cols>
-    <col min="2" max="2" width="29.921875" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="4.3046875" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="4.3828125" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="8.23046875" bestFit="1" customWidth="1"/>
-    <col min="6" max="8" width="7.84375" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="29.9296875" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="4.33203125" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="4.3984375" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="8.19921875" bestFit="1" customWidth="1"/>
+    <col min="6" max="8" width="7.86328125" bestFit="1" customWidth="1"/>
     <col min="9" max="9" width="10" bestFit="1" customWidth="1"/>
-    <col min="10" max="10" width="6.53515625" style="28" customWidth="1"/>
-    <col min="11" max="11" width="10.53515625" bestFit="1" customWidth="1"/>
+    <col min="10" max="10" width="6.53125" style="28" customWidth="1"/>
+    <col min="11" max="11" width="10.53125" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="2:15" ht="12.9" x14ac:dyDescent="0.35">
+    <row r="1" spans="2:15" ht="13.15" x14ac:dyDescent="0.4">
       <c r="B1" s="9"/>
       <c r="C1" s="9"/>
       <c r="D1" s="9"/>
@@ -5433,55 +5426,55 @@
       <c r="F1" s="9"/>
       <c r="G1" s="9"/>
     </row>
-    <row r="2" spans="2:15" ht="12.9" x14ac:dyDescent="0.35">
-      <c r="B2" s="83" t="s">
+    <row r="2" spans="2:15" ht="13.15" x14ac:dyDescent="0.4">
+      <c r="B2" s="75" t="s">
         <v>34</v>
       </c>
-      <c r="C2" s="83"/>
-      <c r="D2" s="83"/>
-      <c r="E2" s="83" t="s">
+      <c r="C2" s="75"/>
+      <c r="D2" s="75"/>
+      <c r="E2" s="75" t="s">
         <v>35</v>
       </c>
-      <c r="F2" s="83">
+      <c r="F2" s="75">
         <v>0.10100000000000001</v>
       </c>
-      <c r="G2" s="83" t="s">
+      <c r="G2" s="75" t="s">
         <v>41</v>
       </c>
     </row>
-    <row r="3" spans="2:15" ht="12.9" x14ac:dyDescent="0.35">
-      <c r="B3" s="83" t="s">
+    <row r="3" spans="2:15" ht="13.15" x14ac:dyDescent="0.4">
+      <c r="B3" s="75" t="s">
         <v>36</v>
       </c>
-      <c r="C3" s="83"/>
-      <c r="D3" s="83"/>
-      <c r="E3" s="83" t="s">
+      <c r="C3" s="75"/>
+      <c r="D3" s="75"/>
+      <c r="E3" s="75" t="s">
         <v>37</v>
       </c>
-      <c r="F3" s="83">
+      <c r="F3" s="75">
         <v>6.3E-2</v>
       </c>
-      <c r="G3" s="83" t="s">
+      <c r="G3" s="75" t="s">
         <v>41</v>
       </c>
     </row>
-    <row r="4" spans="2:15" ht="12.9" x14ac:dyDescent="0.35">
-      <c r="B4" s="83" t="s">
+    <row r="4" spans="2:15" ht="13.15" x14ac:dyDescent="0.4">
+      <c r="B4" s="75" t="s">
         <v>38</v>
       </c>
-      <c r="C4" s="83"/>
-      <c r="D4" s="83"/>
-      <c r="E4" s="83" t="s">
+      <c r="C4" s="75"/>
+      <c r="D4" s="75"/>
+      <c r="E4" s="75" t="s">
         <v>39</v>
       </c>
-      <c r="F4" s="83">
+      <c r="F4" s="75">
         <v>3.6999999999999998E-2</v>
       </c>
-      <c r="G4" s="83" t="s">
+      <c r="G4" s="75" t="s">
         <v>41</v>
       </c>
     </row>
-    <row r="6" spans="2:15" ht="12.9" x14ac:dyDescent="0.35">
+    <row r="6" spans="2:15" ht="13.15" x14ac:dyDescent="0.4">
       <c r="B6" s="2"/>
       <c r="C6" s="2"/>
       <c r="D6" s="2"/>
@@ -5493,7 +5486,7 @@
       <c r="J6" s="16"/>
       <c r="K6" s="9"/>
     </row>
-    <row r="7" spans="2:15" ht="13.3" thickBot="1" x14ac:dyDescent="0.4">
+    <row r="7" spans="2:15" ht="13.5" thickBot="1" x14ac:dyDescent="0.45">
       <c r="B7" s="2"/>
       <c r="C7" s="2"/>
       <c r="D7" s="2"/>
@@ -5512,54 +5505,54 @@
       <c r="J7" s="16"/>
       <c r="K7" s="56"/>
     </row>
-    <row r="8" spans="2:15" ht="12.9" x14ac:dyDescent="0.35">
-      <c r="B8" s="120" t="s">
+    <row r="8" spans="2:15" ht="13.15" x14ac:dyDescent="0.4">
+      <c r="B8" s="111" t="s">
         <v>68</v>
       </c>
-      <c r="C8" s="72"/>
-      <c r="D8" s="72"/>
-      <c r="E8" s="121">
+      <c r="C8" s="70"/>
+      <c r="D8" s="70"/>
+      <c r="E8" s="112">
         <v>21.1</v>
       </c>
-      <c r="F8" s="121">
+      <c r="F8" s="112">
         <v>21.1</v>
       </c>
-      <c r="G8" s="121">
+      <c r="G8" s="112">
         <v>21.1</v>
       </c>
-      <c r="H8" s="121">
+      <c r="H8" s="112">
         <v>21.1</v>
       </c>
       <c r="I8" s="22"/>
       <c r="J8" s="29"/>
       <c r="K8" s="4"/>
     </row>
-    <row r="9" spans="2:15" ht="12.9" x14ac:dyDescent="0.35">
-      <c r="B9" s="99" t="s">
+    <row r="9" spans="2:15" ht="13.15" x14ac:dyDescent="0.4">
+      <c r="B9" s="90" t="s">
         <v>45</v>
       </c>
-      <c r="C9" s="70"/>
-      <c r="D9" s="70"/>
+      <c r="C9" s="68"/>
+      <c r="D9" s="68"/>
       <c r="E9" s="31">
-        <v>66</v>
-      </c>
-      <c r="F9" s="119">
+        <v>132</v>
+      </c>
+      <c r="F9" s="110">
         <f t="shared" ref="F9" si="0">E9</f>
-        <v>66</v>
-      </c>
-      <c r="G9" s="119">
+        <v>132</v>
+      </c>
+      <c r="G9" s="110">
         <f t="shared" ref="G9" si="1">F9</f>
-        <v>66</v>
-      </c>
-      <c r="H9" s="119">
+        <v>132</v>
+      </c>
+      <c r="H9" s="110">
         <f t="shared" ref="H9" si="2">G9</f>
-        <v>66</v>
+        <v>132</v>
       </c>
       <c r="I9" s="23"/>
       <c r="J9" s="30"/>
       <c r="K9" s="5"/>
     </row>
-    <row r="10" spans="2:15" ht="13.3" thickBot="1" x14ac:dyDescent="0.4">
+    <row r="10" spans="2:15" ht="13.5" thickBot="1" x14ac:dyDescent="0.45">
       <c r="B10" s="26" t="s">
         <v>67</v>
       </c>
@@ -5581,118 +5574,145 @@
       <c r="J10" s="30"/>
       <c r="K10" s="5"/>
     </row>
-    <row r="11" spans="2:15" ht="12.9" x14ac:dyDescent="0.35">
-      <c r="B11" s="99" t="s">
+    <row r="11" spans="2:15" ht="13.15" x14ac:dyDescent="0.4">
+      <c r="B11" s="90" t="s">
         <v>66</v>
       </c>
       <c r="C11" s="27"/>
-      <c r="D11" s="94"/>
-      <c r="E11" s="95"/>
-      <c r="F11" s="73"/>
-      <c r="G11" s="73"/>
-      <c r="H11" s="67"/>
+      <c r="D11" s="86"/>
+      <c r="E11" s="87">
+        <v>92.08</v>
+      </c>
+      <c r="F11" s="71">
+        <f>F10*$E$11</f>
+        <v>184.16</v>
+      </c>
+      <c r="G11" s="71">
+        <f>G10*$E$11</f>
+        <v>276.24</v>
+      </c>
+      <c r="H11" s="71">
+        <f>H10*$E$11</f>
+        <v>368.32</v>
+      </c>
       <c r="I11" s="66"/>
       <c r="J11" s="30"/>
       <c r="K11" s="5"/>
     </row>
-    <row r="12" spans="2:15" ht="12.9" x14ac:dyDescent="0.35">
-      <c r="B12" s="99" t="s">
+    <row r="12" spans="2:15" ht="13.15" x14ac:dyDescent="0.4">
+      <c r="B12" s="90" t="s">
         <v>65</v>
       </c>
       <c r="C12" s="27"/>
-      <c r="D12" s="94"/>
-      <c r="E12" s="96"/>
-      <c r="F12" s="90"/>
-      <c r="G12" s="90"/>
-      <c r="H12" s="91"/>
+      <c r="D12" s="86"/>
+      <c r="E12" s="88">
+        <v>1</v>
+      </c>
+      <c r="F12" s="82">
+        <v>1</v>
+      </c>
+      <c r="G12" s="82">
+        <v>1</v>
+      </c>
+      <c r="H12" s="83">
+        <v>1</v>
+      </c>
       <c r="I12" s="66"/>
       <c r="J12" s="30"/>
       <c r="K12" s="5"/>
     </row>
-    <row r="13" spans="2:15" ht="13.3" thickBot="1" x14ac:dyDescent="0.4">
-      <c r="B13" s="122" t="s">
+    <row r="13" spans="2:15" ht="13.5" thickBot="1" x14ac:dyDescent="0.45">
+      <c r="B13" s="113" t="s">
         <v>50</v>
       </c>
-      <c r="C13" s="74"/>
-      <c r="D13" s="123"/>
-      <c r="E13" s="97"/>
-      <c r="F13" s="68"/>
-      <c r="G13" s="68"/>
-      <c r="H13" s="69"/>
-      <c r="I13" s="124"/>
-      <c r="J13" s="103"/>
-      <c r="K13" s="104"/>
-    </row>
-    <row r="14" spans="2:15" ht="12.9" x14ac:dyDescent="0.35">
+      <c r="C13" s="72"/>
+      <c r="D13" s="114"/>
+      <c r="E13" s="89">
+        <v>0.10100000000000001</v>
+      </c>
+      <c r="F13" s="67">
+        <v>0.10100000000000001</v>
+      </c>
+      <c r="G13" s="67">
+        <v>0.10100000000000001</v>
+      </c>
+      <c r="H13" s="67">
+        <v>0.10100000000000001</v>
+      </c>
+      <c r="I13" s="115"/>
+      <c r="J13" s="94"/>
+      <c r="K13" s="95"/>
+    </row>
+    <row r="14" spans="2:15" ht="13.15" x14ac:dyDescent="0.4">
       <c r="B14" s="21"/>
-      <c r="C14" s="71"/>
-      <c r="D14" s="71"/>
-      <c r="E14" s="109" t="s">
+      <c r="C14" s="69"/>
+      <c r="D14" s="69"/>
+      <c r="E14" s="100" t="s">
         <v>40</v>
       </c>
-      <c r="F14" s="109" t="s">
+      <c r="F14" s="100" t="s">
         <v>40</v>
       </c>
-      <c r="G14" s="109" t="s">
+      <c r="G14" s="100" t="s">
         <v>40</v>
       </c>
-      <c r="H14" s="109" t="s">
+      <c r="H14" s="100" t="s">
         <v>40</v>
       </c>
       <c r="I14" s="23"/>
       <c r="J14" s="30"/>
       <c r="K14" s="5"/>
     </row>
-    <row r="15" spans="2:15" ht="13.3" thickBot="1" x14ac:dyDescent="0.4">
-      <c r="B15" s="100" t="s">
+    <row r="15" spans="2:15" ht="13.5" thickBot="1" x14ac:dyDescent="0.45">
+      <c r="B15" s="91" t="s">
         <v>46</v>
       </c>
-      <c r="C15" s="101"/>
-      <c r="D15" s="101"/>
-      <c r="E15" s="102">
+      <c r="C15" s="92"/>
+      <c r="D15" s="92"/>
+      <c r="E15" s="93">
         <v>2.5</v>
       </c>
-      <c r="F15" s="102">
+      <c r="F15" s="93">
         <v>2.5</v>
       </c>
-      <c r="G15" s="102">
+      <c r="G15" s="93">
         <v>2</v>
       </c>
-      <c r="H15" s="102">
+      <c r="H15" s="93">
         <v>1.5</v>
       </c>
-      <c r="I15" s="102"/>
-      <c r="J15" s="103"/>
-      <c r="K15" s="104"/>
-    </row>
-    <row r="16" spans="2:15" ht="13.3" thickBot="1" x14ac:dyDescent="0.4">
-      <c r="B16" s="106" t="s">
+      <c r="I15" s="93"/>
+      <c r="J15" s="94"/>
+      <c r="K15" s="95"/>
+    </row>
+    <row r="16" spans="2:15" ht="13.5" thickBot="1" x14ac:dyDescent="0.45">
+      <c r="B16" s="97" t="s">
         <v>62</v>
       </c>
-      <c r="C16" s="105" t="s">
+      <c r="C16" s="96" t="s">
         <v>63</v>
       </c>
-      <c r="D16" s="98"/>
+      <c r="D16" s="76"/>
       <c r="E16" s="29"/>
       <c r="F16" s="23"/>
       <c r="G16" s="23"/>
       <c r="H16" s="23"/>
-      <c r="I16" s="110" t="s">
+      <c r="I16" s="101" t="s">
         <v>15</v>
       </c>
-      <c r="J16" s="111" t="s">
+      <c r="J16" s="102" t="s">
         <v>0</v>
       </c>
-      <c r="K16" s="112" t="s">
+      <c r="K16" s="103" t="s">
         <v>44</v>
       </c>
-      <c r="O16" s="118"/>
-    </row>
-    <row r="17" spans="2:11" ht="12.9" x14ac:dyDescent="0.35">
-      <c r="B17" s="107" t="s">
+      <c r="O16" s="109"/>
+    </row>
+    <row r="17" spans="2:11" ht="13.15" x14ac:dyDescent="0.4">
+      <c r="B17" s="98" t="s">
         <v>1</v>
       </c>
-      <c r="C17" s="108" t="s">
+      <c r="C17" s="99" t="s">
         <v>43</v>
       </c>
       <c r="D17" s="63" t="s">
@@ -5702,15 +5722,15 @@
       <c r="F17" s="24"/>
       <c r="G17" s="24"/>
       <c r="H17" s="24"/>
-      <c r="I17" s="113" t="s">
+      <c r="I17" s="104" t="s">
         <v>47</v>
       </c>
-      <c r="J17" s="114"/>
-      <c r="K17" s="115" t="s">
+      <c r="J17" s="105"/>
+      <c r="K17" s="106" t="s">
         <v>48</v>
       </c>
     </row>
-    <row r="18" spans="2:11" ht="12.9" x14ac:dyDescent="0.35">
+    <row r="18" spans="2:11" ht="13.15" x14ac:dyDescent="0.4">
       <c r="B18" s="20">
         <v>0.5</v>
       </c>
@@ -5718,7 +5738,10 @@
         <f>'WTG Yield Wake'!D14</f>
         <v>0</v>
       </c>
-      <c r="D18" s="64"/>
+      <c r="D18" s="64">
+        <f>C18/0.95</f>
+        <v>0</v>
+      </c>
       <c r="E18" s="62">
         <v>0</v>
       </c>
@@ -5738,12 +5761,12 @@
       <c r="J18" s="32">
         <v>57</v>
       </c>
-      <c r="K18" s="116">
+      <c r="K18" s="107">
         <f>I18*J18/1000</f>
         <v>0</v>
       </c>
     </row>
-    <row r="19" spans="2:11" ht="12.9" x14ac:dyDescent="0.35">
+    <row r="19" spans="2:11" ht="13.15" x14ac:dyDescent="0.4">
       <c r="B19" s="20">
         <v>1.5</v>
       </c>
@@ -5751,7 +5774,10 @@
         <f>'WTG Yield Wake'!D15</f>
         <v>0</v>
       </c>
-      <c r="D19" s="64"/>
+      <c r="D19" s="64">
+        <f t="shared" ref="D19:D45" si="3">C19/0.95</f>
+        <v>0</v>
+      </c>
       <c r="E19" s="62">
         <v>0</v>
       </c>
@@ -5765,19 +5791,19 @@
         <v>0</v>
       </c>
       <c r="I19" s="58">
-        <f t="shared" ref="I19:I46" si="3">SUM(E19:H19)</f>
+        <f t="shared" ref="I19:I46" si="4">SUM(E19:H19)</f>
         <v>0</v>
       </c>
       <c r="J19" s="32">
         <f>'WTG Yield Wake'!I15*8760/100</f>
         <v>151.98599999999999</v>
       </c>
-      <c r="K19" s="116">
-        <f t="shared" ref="K19:K46" si="4">I19*J19/1000</f>
+      <c r="K19" s="107">
+        <f t="shared" ref="K19:K46" si="5">I19*J19/1000</f>
         <v>0</v>
       </c>
     </row>
-    <row r="20" spans="2:11" ht="12.9" x14ac:dyDescent="0.35">
+    <row r="20" spans="2:11" ht="13.15" x14ac:dyDescent="0.4">
       <c r="B20" s="20">
         <v>2.5</v>
       </c>
@@ -5785,7 +5811,10 @@
         <f>'WTG Yield Wake'!D16</f>
         <v>0</v>
       </c>
-      <c r="D20" s="64"/>
+      <c r="D20" s="64">
+        <f t="shared" si="3"/>
+        <v>0</v>
+      </c>
       <c r="E20" s="62">
         <v>0</v>
       </c>
@@ -5799,19 +5828,19 @@
         <v>0</v>
       </c>
       <c r="I20" s="58">
-        <f t="shared" si="3"/>
+        <f t="shared" si="4"/>
         <v>0</v>
       </c>
       <c r="J20" s="32">
         <f>'WTG Yield Wake'!I16*8760/100</f>
         <v>293.98559999999998</v>
       </c>
-      <c r="K20" s="116">
-        <f t="shared" si="4"/>
+      <c r="K20" s="107">
+        <f t="shared" si="5"/>
         <v>0</v>
       </c>
     </row>
-    <row r="21" spans="2:11" ht="12.9" x14ac:dyDescent="0.35">
+    <row r="21" spans="2:11" ht="13.15" x14ac:dyDescent="0.4">
       <c r="B21" s="20">
         <v>3.5</v>
       </c>
@@ -5819,37 +5848,40 @@
         <f>'WTG Yield Wake'!D17</f>
         <v>0.437</v>
       </c>
-      <c r="D21" s="64"/>
+      <c r="D21" s="64">
+        <f t="shared" si="3"/>
+        <v>0.46</v>
+      </c>
       <c r="E21" s="62">
         <f>3*($D21/E$8*E$11)^2*E$13*E$15/1000</f>
-        <v>0</v>
+        <v>3.0525586093681635E-3</v>
       </c>
       <c r="F21" s="57">
-        <f t="shared" ref="F21:H36" si="5">3*($D21/F$8*F$11)^2*F$13*F$15/1000</f>
-        <v>0</v>
+        <f t="shared" ref="F21:H36" si="6">3*($D21/F$8*F$11)^2*F$13*F$15/1000</f>
+        <v>1.2210234437472654E-2</v>
       </c>
       <c r="G21" s="57">
-        <f t="shared" si="5"/>
-        <v>0</v>
+        <f t="shared" si="6"/>
+        <v>2.1978421987450775E-2</v>
       </c>
       <c r="H21" s="57">
-        <f t="shared" si="5"/>
-        <v>0</v>
+        <f t="shared" si="6"/>
+        <v>2.9304562649934369E-2</v>
       </c>
       <c r="I21" s="58">
-        <f t="shared" si="3"/>
-        <v>0</v>
+        <f t="shared" si="4"/>
+        <v>6.6545777684225954E-2</v>
       </c>
       <c r="J21" s="32">
         <f>'WTG Yield Wake'!I17*8760/100</f>
         <v>423.28320000000002</v>
       </c>
-      <c r="K21" s="116">
-        <f t="shared" si="4"/>
-        <v>0</v>
-      </c>
-    </row>
-    <row r="22" spans="2:11" ht="12.9" x14ac:dyDescent="0.35">
+      <c r="K21" s="107">
+        <f t="shared" si="5"/>
+        <v>2.8167709724667752E-2</v>
+      </c>
+    </row>
+    <row r="22" spans="2:11" ht="13.15" x14ac:dyDescent="0.4">
       <c r="B22" s="20">
         <v>4.5</v>
       </c>
@@ -5857,37 +5889,40 @@
         <f>'WTG Yield Wake'!D18</f>
         <v>1.423</v>
       </c>
-      <c r="D22" s="64"/>
+      <c r="D22" s="64">
+        <f t="shared" si="3"/>
+        <v>1.4978947368421054</v>
+      </c>
       <c r="E22" s="62">
-        <f t="shared" ref="E22:H46" si="6">3*($D22/E$8*E$11)^2*E$13*E$15/1000</f>
-        <v>0</v>
+        <f t="shared" ref="E22:H46" si="7">3*($D22/E$8*E$11)^2*E$13*E$15/1000</f>
+        <v>3.2367632716876912E-2</v>
       </c>
       <c r="F22" s="57">
-        <f t="shared" si="5"/>
-        <v>0</v>
+        <f t="shared" si="6"/>
+        <v>0.12947053086750765</v>
       </c>
       <c r="G22" s="57">
-        <f t="shared" si="5"/>
-        <v>0</v>
+        <f t="shared" si="6"/>
+        <v>0.23304695556151375</v>
       </c>
       <c r="H22" s="57">
-        <f t="shared" si="5"/>
-        <v>0</v>
+        <f t="shared" si="6"/>
+        <v>0.31072927408201839</v>
       </c>
       <c r="I22" s="58">
-        <f t="shared" si="3"/>
-        <v>0</v>
+        <f t="shared" si="4"/>
+        <v>0.70561439322791664</v>
       </c>
       <c r="J22" s="32">
         <f>'WTG Yield Wake'!I18*8760/100</f>
         <v>559.7639999999999</v>
       </c>
-      <c r="K22" s="116">
-        <f t="shared" si="4"/>
-        <v>0</v>
-      </c>
-    </row>
-    <row r="23" spans="2:11" ht="12.9" x14ac:dyDescent="0.35">
+      <c r="K22" s="107">
+        <f t="shared" si="5"/>
+        <v>0.39497753521083145</v>
+      </c>
+    </row>
+    <row r="23" spans="2:11" ht="13.15" x14ac:dyDescent="0.4">
       <c r="B23" s="20">
         <v>5.5</v>
       </c>
@@ -5895,37 +5930,40 @@
         <f>'WTG Yield Wake'!D19</f>
         <v>2.83</v>
       </c>
-      <c r="D23" s="64"/>
+      <c r="D23" s="64">
+        <f t="shared" si="3"/>
+        <v>2.978947368421053</v>
+      </c>
       <c r="E23" s="62">
+        <f t="shared" si="7"/>
+        <v>0.12801887555869634</v>
+      </c>
+      <c r="F23" s="57">
         <f t="shared" si="6"/>
-        <v>0</v>
-      </c>
-      <c r="F23" s="57">
-        <f t="shared" si="5"/>
-        <v>0</v>
+        <v>0.51207550223478537</v>
       </c>
       <c r="G23" s="57">
-        <f t="shared" si="5"/>
-        <v>0</v>
+        <f t="shared" si="6"/>
+        <v>0.92173590402261363</v>
       </c>
       <c r="H23" s="57">
-        <f t="shared" si="5"/>
-        <v>0</v>
+        <f t="shared" si="6"/>
+        <v>1.228981205363485</v>
       </c>
       <c r="I23" s="58">
-        <f t="shared" si="3"/>
-        <v>0</v>
+        <f t="shared" si="4"/>
+        <v>2.7908114871795804</v>
       </c>
       <c r="J23" s="32">
         <f>'WTG Yield Wake'!I19*8760/100</f>
         <v>670.75320000000011</v>
       </c>
-      <c r="K23" s="116">
-        <f t="shared" si="4"/>
-        <v>0</v>
-      </c>
-    </row>
-    <row r="24" spans="2:11" ht="12.9" x14ac:dyDescent="0.35">
+      <c r="K23" s="107">
+        <f t="shared" si="5"/>
+        <v>1.8719457356224627</v>
+      </c>
+    </row>
+    <row r="24" spans="2:11" ht="13.15" x14ac:dyDescent="0.4">
       <c r="B24" s="20">
         <v>6.5</v>
       </c>
@@ -5933,37 +5971,40 @@
         <f>'WTG Yield Wake'!D20</f>
         <v>4.7720000000000002</v>
       </c>
-      <c r="D24" s="64"/>
+      <c r="D24" s="64">
+        <f t="shared" si="3"/>
+        <v>5.0231578947368423</v>
+      </c>
       <c r="E24" s="62">
+        <f t="shared" si="7"/>
+        <v>0.36400052265862032</v>
+      </c>
+      <c r="F24" s="57">
         <f t="shared" si="6"/>
-        <v>0</v>
-      </c>
-      <c r="F24" s="57">
-        <f t="shared" si="5"/>
-        <v>0</v>
+        <v>1.4560020906344813</v>
       </c>
       <c r="G24" s="57">
-        <f t="shared" si="5"/>
-        <v>0</v>
+        <f t="shared" si="6"/>
+        <v>2.6208037631420664</v>
       </c>
       <c r="H24" s="57">
-        <f t="shared" si="5"/>
-        <v>0</v>
+        <f t="shared" si="6"/>
+        <v>3.4944050175227548</v>
       </c>
       <c r="I24" s="58">
-        <f t="shared" si="3"/>
-        <v>0</v>
+        <f t="shared" si="4"/>
+        <v>7.935211393957923</v>
       </c>
       <c r="J24" s="32">
         <f>'WTG Yield Wake'!I20*8760/100</f>
         <v>764.92319999999995</v>
       </c>
-      <c r="K24" s="116">
-        <f t="shared" si="4"/>
-        <v>0</v>
-      </c>
-    </row>
-    <row r="25" spans="2:11" ht="12.9" x14ac:dyDescent="0.35">
+      <c r="K24" s="107">
+        <f t="shared" si="5"/>
+        <v>6.0698272921427554</v>
+      </c>
+    </row>
+    <row r="25" spans="2:11" ht="13.15" x14ac:dyDescent="0.4">
       <c r="B25" s="20">
         <v>7.5</v>
       </c>
@@ -5971,37 +6012,40 @@
         <f>'WTG Yield Wake'!D21</f>
         <v>7.46</v>
       </c>
-      <c r="D25" s="64"/>
+      <c r="D25" s="64">
+        <f t="shared" si="3"/>
+        <v>7.8526315789473689</v>
+      </c>
       <c r="E25" s="62">
+        <f t="shared" si="7"/>
+        <v>0.88956726329987201</v>
+      </c>
+      <c r="F25" s="57">
         <f t="shared" si="6"/>
-        <v>0</v>
-      </c>
-      <c r="F25" s="57">
-        <f t="shared" si="5"/>
-        <v>0</v>
+        <v>3.5582690531994881</v>
       </c>
       <c r="G25" s="57">
-        <f t="shared" si="5"/>
-        <v>0</v>
+        <f t="shared" si="6"/>
+        <v>6.4048842957590795</v>
       </c>
       <c r="H25" s="57">
-        <f t="shared" si="5"/>
-        <v>0</v>
+        <f t="shared" si="6"/>
+        <v>8.539845727678772</v>
       </c>
       <c r="I25" s="58">
-        <f t="shared" si="3"/>
-        <v>0</v>
+        <f t="shared" si="4"/>
+        <v>19.392566339937211</v>
       </c>
       <c r="J25" s="32">
         <f>'WTG Yield Wake'!I21*8760/100</f>
         <v>827.64480000000015</v>
       </c>
-      <c r="K25" s="116">
-        <f t="shared" si="4"/>
-        <v>0</v>
-      </c>
-    </row>
-    <row r="26" spans="2:11" ht="12.9" x14ac:dyDescent="0.35">
+      <c r="K25" s="107">
+        <f t="shared" si="5"/>
+        <v>16.050156689904068</v>
+      </c>
+    </row>
+    <row r="26" spans="2:11" ht="13.15" x14ac:dyDescent="0.4">
       <c r="B26" s="20">
         <v>8.5</v>
       </c>
@@ -6009,37 +6053,40 @@
         <f>'WTG Yield Wake'!D22</f>
         <v>10.949</v>
       </c>
-      <c r="D26" s="64"/>
+      <c r="D26" s="64">
+        <f t="shared" si="3"/>
+        <v>11.525263157894738</v>
+      </c>
       <c r="E26" s="62">
+        <f t="shared" si="7"/>
+        <v>1.9162406499420312</v>
+      </c>
+      <c r="F26" s="57">
         <f t="shared" si="6"/>
-        <v>0</v>
-      </c>
-      <c r="F26" s="57">
-        <f t="shared" si="5"/>
-        <v>0</v>
+        <v>7.664962599768125</v>
       </c>
       <c r="G26" s="57">
-        <f t="shared" si="5"/>
-        <v>0</v>
+        <f t="shared" si="6"/>
+        <v>13.796932679582625</v>
       </c>
       <c r="H26" s="57">
-        <f t="shared" si="5"/>
-        <v>0</v>
+        <f t="shared" si="6"/>
+        <v>18.395910239443502</v>
       </c>
       <c r="I26" s="58">
-        <f t="shared" si="3"/>
-        <v>0</v>
+        <f t="shared" si="4"/>
+        <v>41.774046168736284</v>
       </c>
       <c r="J26" s="32">
         <f>'WTG Yield Wake'!I22*8760/100</f>
         <v>842.62440000000004</v>
       </c>
-      <c r="K26" s="116">
-        <f t="shared" si="4"/>
-        <v>0</v>
-      </c>
-    </row>
-    <row r="27" spans="2:11" ht="12.9" x14ac:dyDescent="0.35">
+      <c r="K26" s="107">
+        <f t="shared" si="5"/>
+        <v>35.199830588503708</v>
+      </c>
+    </row>
+    <row r="27" spans="2:11" ht="13.15" x14ac:dyDescent="0.4">
       <c r="B27" s="20">
         <v>9.5</v>
       </c>
@@ -6047,37 +6094,40 @@
         <f>'WTG Yield Wake'!D23</f>
         <v>14.622999999999999</v>
       </c>
-      <c r="D27" s="64"/>
+      <c r="D27" s="64">
+        <f t="shared" si="3"/>
+        <v>15.392631578947368</v>
+      </c>
       <c r="E27" s="62">
+        <f t="shared" si="7"/>
+        <v>3.4180160462612976</v>
+      </c>
+      <c r="F27" s="57">
         <f t="shared" si="6"/>
-        <v>0</v>
-      </c>
-      <c r="F27" s="57">
-        <f t="shared" si="5"/>
-        <v>0</v>
+        <v>13.67206418504519</v>
       </c>
       <c r="G27" s="57">
-        <f t="shared" si="5"/>
-        <v>0</v>
+        <f t="shared" si="6"/>
+        <v>24.609715533081339</v>
       </c>
       <c r="H27" s="57">
-        <f t="shared" si="5"/>
-        <v>0</v>
+        <f t="shared" si="6"/>
+        <v>32.812954044108452</v>
       </c>
       <c r="I27" s="58">
-        <f t="shared" si="3"/>
-        <v>0</v>
+        <f t="shared" si="4"/>
+        <v>74.512749808496281</v>
       </c>
       <c r="J27" s="32">
         <f>'WTG Yield Wake'!I23*8760/100</f>
         <v>799.1748</v>
       </c>
-      <c r="K27" s="116">
-        <f t="shared" si="4"/>
-        <v>0</v>
-      </c>
-    </row>
-    <row r="28" spans="2:11" ht="12.9" x14ac:dyDescent="0.35">
+      <c r="K27" s="107">
+        <f t="shared" si="5"/>
+        <v>59.548711925655049</v>
+      </c>
+    </row>
+    <row r="28" spans="2:11" ht="13.15" x14ac:dyDescent="0.4">
       <c r="B28" s="20">
         <v>10.5</v>
       </c>
@@ -6085,37 +6135,40 @@
         <f>'WTG Yield Wake'!D24</f>
         <v>17.73</v>
       </c>
-      <c r="D28" s="64"/>
+      <c r="D28" s="64">
+        <f t="shared" si="3"/>
+        <v>18.663157894736845</v>
+      </c>
       <c r="E28" s="62">
+        <f t="shared" si="7"/>
+        <v>5.0247980105401906</v>
+      </c>
+      <c r="F28" s="57">
         <f t="shared" si="6"/>
-        <v>0</v>
-      </c>
-      <c r="F28" s="57">
-        <f t="shared" si="5"/>
-        <v>0</v>
+        <v>20.099192042160762</v>
       </c>
       <c r="G28" s="57">
-        <f t="shared" si="5"/>
-        <v>0</v>
+        <f t="shared" si="6"/>
+        <v>36.178545675889367</v>
       </c>
       <c r="H28" s="57">
-        <f t="shared" si="5"/>
-        <v>0</v>
+        <f t="shared" si="6"/>
+        <v>48.238060901185833</v>
       </c>
       <c r="I28" s="58">
-        <f t="shared" si="3"/>
-        <v>0</v>
+        <f t="shared" si="4"/>
+        <v>109.54059662977616</v>
       </c>
       <c r="J28" s="32">
         <f>'WTG Yield Wake'!I24*8760/100</f>
         <v>717.61919999999998</v>
       </c>
-      <c r="K28" s="116">
-        <f t="shared" si="4"/>
-        <v>0</v>
-      </c>
-    </row>
-    <row r="29" spans="2:11" ht="12.9" x14ac:dyDescent="0.35">
+      <c r="K28" s="107">
+        <f t="shared" si="5"/>
+        <v>78.608435320982665</v>
+      </c>
+    </row>
+    <row r="29" spans="2:11" ht="13.15" x14ac:dyDescent="0.4">
       <c r="B29" s="20">
         <v>11.5</v>
       </c>
@@ -6123,37 +6176,40 @@
         <f>'WTG Yield Wake'!D25</f>
         <v>19.442</v>
       </c>
-      <c r="D29" s="64"/>
+      <c r="D29" s="64">
+        <f t="shared" si="3"/>
+        <v>20.465263157894739</v>
+      </c>
       <c r="E29" s="62">
+        <f t="shared" si="7"/>
+        <v>6.042031913268727</v>
+      </c>
+      <c r="F29" s="57">
         <f t="shared" si="6"/>
-        <v>0</v>
-      </c>
-      <c r="F29" s="57">
-        <f t="shared" si="5"/>
-        <v>0</v>
+        <v>24.168127653074908</v>
       </c>
       <c r="G29" s="57">
-        <f t="shared" si="5"/>
-        <v>0</v>
+        <f t="shared" si="6"/>
+        <v>43.502629775534828</v>
       </c>
       <c r="H29" s="57">
-        <f t="shared" si="5"/>
-        <v>0</v>
+        <f t="shared" si="6"/>
+        <v>58.003506367379778</v>
       </c>
       <c r="I29" s="58">
-        <f t="shared" si="3"/>
-        <v>0</v>
+        <f t="shared" si="4"/>
+        <v>131.71629570925825</v>
       </c>
       <c r="J29" s="32">
         <f>'WTG Yield Wake'!I25*8760/100</f>
         <v>620.38319999999999</v>
       </c>
-      <c r="K29" s="116">
-        <f t="shared" si="4"/>
-        <v>0</v>
-      </c>
-    </row>
-    <row r="30" spans="2:11" ht="12.9" x14ac:dyDescent="0.35">
+      <c r="K29" s="107">
+        <f t="shared" si="5"/>
+        <v>81.714577024255888</v>
+      </c>
+    </row>
+    <row r="30" spans="2:11" ht="13.15" x14ac:dyDescent="0.4">
       <c r="B30" s="20">
         <v>12.5</v>
       </c>
@@ -6161,37 +6217,40 @@
         <f>'WTG Yield Wake'!D26</f>
         <v>19.920999999999999</v>
       </c>
-      <c r="D30" s="64"/>
+      <c r="D30" s="64">
+        <f t="shared" si="3"/>
+        <v>20.969473684210527</v>
+      </c>
       <c r="E30" s="62">
+        <f t="shared" si="7"/>
+        <v>6.3434191390222656</v>
+      </c>
+      <c r="F30" s="57">
         <f t="shared" si="6"/>
-        <v>0</v>
-      </c>
-      <c r="F30" s="57">
-        <f t="shared" si="5"/>
-        <v>0</v>
+        <v>25.373676556089062</v>
       </c>
       <c r="G30" s="57">
-        <f t="shared" si="5"/>
-        <v>0</v>
+        <f t="shared" si="6"/>
+        <v>45.67261780096031</v>
       </c>
       <c r="H30" s="57">
-        <f t="shared" si="5"/>
-        <v>0</v>
+        <f t="shared" si="6"/>
+        <v>60.896823734613747</v>
       </c>
       <c r="I30" s="58">
-        <f t="shared" si="3"/>
-        <v>0</v>
+        <f t="shared" si="4"/>
+        <v>138.28653723068538</v>
       </c>
       <c r="J30" s="32">
         <f>'WTG Yield Wake'!I26*8760/100</f>
         <v>510.27</v>
       </c>
-      <c r="K30" s="116">
-        <f t="shared" si="4"/>
-        <v>0</v>
-      </c>
-    </row>
-    <row r="31" spans="2:11" ht="12.9" x14ac:dyDescent="0.35">
+      <c r="K30" s="107">
+        <f t="shared" si="5"/>
+        <v>70.563471352701839</v>
+      </c>
+    </row>
+    <row r="31" spans="2:11" ht="13.15" x14ac:dyDescent="0.4">
       <c r="B31" s="20">
         <v>13.5</v>
       </c>
@@ -6199,37 +6258,40 @@
         <f>'WTG Yield Wake'!D27</f>
         <v>19.991</v>
       </c>
-      <c r="D31" s="64"/>
+      <c r="D31" s="64">
+        <f t="shared" si="3"/>
+        <v>21.043157894736844</v>
+      </c>
       <c r="E31" s="62">
+        <f t="shared" si="7"/>
+        <v>6.3880774885198131</v>
+      </c>
+      <c r="F31" s="57">
         <f t="shared" si="6"/>
-        <v>0</v>
-      </c>
-      <c r="F31" s="57">
-        <f t="shared" si="5"/>
-        <v>0</v>
+        <v>25.552309954079252</v>
       </c>
       <c r="G31" s="57">
-        <f t="shared" si="5"/>
-        <v>0</v>
+        <f t="shared" si="6"/>
+        <v>45.994157917342662</v>
       </c>
       <c r="H31" s="57">
-        <f t="shared" si="5"/>
-        <v>0</v>
+        <f t="shared" si="6"/>
+        <v>61.325543889790211</v>
       </c>
       <c r="I31" s="58">
-        <f t="shared" si="3"/>
-        <v>0</v>
+        <f t="shared" si="4"/>
+        <v>139.26008924973195</v>
       </c>
       <c r="J31" s="32">
         <f>'WTG Yield Wake'!I27*8760/100</f>
         <v>399.2808</v>
       </c>
-      <c r="K31" s="116">
-        <f t="shared" si="4"/>
-        <v>0</v>
-      </c>
-    </row>
-    <row r="32" spans="2:11" ht="12.9" x14ac:dyDescent="0.35">
+      <c r="K31" s="107">
+        <f t="shared" si="5"/>
+        <v>55.603879843704377</v>
+      </c>
+    </row>
+    <row r="32" spans="2:11" ht="13.15" x14ac:dyDescent="0.4">
       <c r="B32" s="20">
         <v>14.5</v>
       </c>
@@ -6237,37 +6299,40 @@
         <f>'WTG Yield Wake'!D28</f>
         <v>20</v>
       </c>
-      <c r="D32" s="64"/>
+      <c r="D32" s="64">
+        <f t="shared" si="3"/>
+        <v>21.05263157894737</v>
+      </c>
       <c r="E32" s="62">
+        <f t="shared" si="7"/>
+        <v>6.3938306413463195</v>
+      </c>
+      <c r="F32" s="57">
         <f t="shared" si="6"/>
-        <v>0</v>
-      </c>
-      <c r="F32" s="57">
-        <f t="shared" si="5"/>
-        <v>0</v>
+        <v>25.575322565385278</v>
       </c>
       <c r="G32" s="57">
-        <f t="shared" si="5"/>
-        <v>0</v>
+        <f t="shared" si="6"/>
+        <v>46.035580617693491</v>
       </c>
       <c r="H32" s="57">
-        <f t="shared" si="5"/>
-        <v>0</v>
+        <f t="shared" si="6"/>
+        <v>61.380774156924666</v>
       </c>
       <c r="I32" s="58">
-        <f t="shared" si="3"/>
-        <v>0</v>
+        <f t="shared" si="4"/>
+        <v>139.38550798134975</v>
       </c>
       <c r="J32" s="32">
         <f>'WTG Yield Wake'!I28*8760/100</f>
         <v>295.47480000000002</v>
       </c>
-      <c r="K32" s="116">
-        <f t="shared" si="4"/>
-        <v>0</v>
-      </c>
-    </row>
-    <row r="33" spans="1:13" ht="12.9" x14ac:dyDescent="0.35">
+      <c r="K32" s="107">
+        <f t="shared" si="5"/>
+        <v>41.184905093687725</v>
+      </c>
+    </row>
+    <row r="33" spans="1:13" ht="13.15" x14ac:dyDescent="0.4">
       <c r="B33" s="20">
         <v>15.5</v>
       </c>
@@ -6275,37 +6340,40 @@
         <f>'WTG Yield Wake'!D29</f>
         <v>20</v>
       </c>
-      <c r="D33" s="64"/>
+      <c r="D33" s="64">
+        <f t="shared" si="3"/>
+        <v>21.05263157894737</v>
+      </c>
       <c r="E33" s="62">
+        <f t="shared" si="7"/>
+        <v>6.3938306413463195</v>
+      </c>
+      <c r="F33" s="57">
         <f t="shared" si="6"/>
-        <v>0</v>
-      </c>
-      <c r="F33" s="57">
-        <f t="shared" si="5"/>
-        <v>0</v>
+        <v>25.575322565385278</v>
       </c>
       <c r="G33" s="57">
-        <f t="shared" si="5"/>
-        <v>0</v>
+        <f t="shared" si="6"/>
+        <v>46.035580617693491</v>
       </c>
       <c r="H33" s="57">
-        <f t="shared" si="5"/>
-        <v>0</v>
+        <f t="shared" si="6"/>
+        <v>61.380774156924666</v>
       </c>
       <c r="I33" s="58">
-        <f t="shared" si="3"/>
-        <v>0</v>
+        <f t="shared" si="4"/>
+        <v>139.38550798134975</v>
       </c>
       <c r="J33" s="32">
         <f>'WTG Yield Wake'!I29*8760/100</f>
         <v>211.46640000000002</v>
       </c>
-      <c r="K33" s="116">
-        <f t="shared" si="4"/>
-        <v>0</v>
-      </c>
-    </row>
-    <row r="34" spans="1:13" ht="12.9" x14ac:dyDescent="0.35">
+      <c r="K33" s="107">
+        <f t="shared" si="5"/>
+        <v>29.475351584987301</v>
+      </c>
+    </row>
+    <row r="34" spans="1:13" ht="13.15" x14ac:dyDescent="0.4">
       <c r="B34" s="20">
         <v>16.5</v>
       </c>
@@ -6313,37 +6381,40 @@
         <f>'WTG Yield Wake'!D30</f>
         <v>20</v>
       </c>
-      <c r="D34" s="64"/>
+      <c r="D34" s="64">
+        <f t="shared" si="3"/>
+        <v>21.05263157894737</v>
+      </c>
       <c r="E34" s="62">
+        <f t="shared" si="7"/>
+        <v>6.3938306413463195</v>
+      </c>
+      <c r="F34" s="57">
         <f t="shared" si="6"/>
-        <v>0</v>
-      </c>
-      <c r="F34" s="57">
-        <f t="shared" si="5"/>
-        <v>0</v>
+        <v>25.575322565385278</v>
       </c>
       <c r="G34" s="57">
-        <f t="shared" si="5"/>
-        <v>0</v>
+        <f t="shared" si="6"/>
+        <v>46.035580617693491</v>
       </c>
       <c r="H34" s="57">
-        <f t="shared" si="5"/>
-        <v>0</v>
+        <f t="shared" si="6"/>
+        <v>61.380774156924666</v>
       </c>
       <c r="I34" s="58">
-        <f t="shared" si="3"/>
-        <v>0</v>
+        <f t="shared" si="4"/>
+        <v>139.38550798134975</v>
       </c>
       <c r="J34" s="32">
         <f>'WTG Yield Wake'!I30*8760/100</f>
         <v>157.76760000000002</v>
       </c>
-      <c r="K34" s="116">
-        <f t="shared" si="4"/>
-        <v>0</v>
-      </c>
-    </row>
-    <row r="35" spans="1:13" ht="12.9" x14ac:dyDescent="0.35">
+      <c r="K34" s="107">
+        <f t="shared" si="5"/>
+        <v>21.990517068998397</v>
+      </c>
+    </row>
+    <row r="35" spans="1:13" ht="13.15" x14ac:dyDescent="0.4">
       <c r="B35" s="20">
         <v>17.5</v>
       </c>
@@ -6351,37 +6422,40 @@
         <f>'WTG Yield Wake'!D31</f>
         <v>20</v>
       </c>
-      <c r="D35" s="64"/>
+      <c r="D35" s="64">
+        <f t="shared" si="3"/>
+        <v>21.05263157894737</v>
+      </c>
       <c r="E35" s="62">
+        <f t="shared" si="7"/>
+        <v>6.3938306413463195</v>
+      </c>
+      <c r="F35" s="57">
         <f t="shared" si="6"/>
-        <v>0</v>
-      </c>
-      <c r="F35" s="57">
-        <f t="shared" si="5"/>
-        <v>0</v>
+        <v>25.575322565385278</v>
       </c>
       <c r="G35" s="57">
-        <f t="shared" si="5"/>
-        <v>0</v>
+        <f t="shared" si="6"/>
+        <v>46.035580617693491</v>
       </c>
       <c r="H35" s="57">
-        <f t="shared" si="5"/>
-        <v>0</v>
+        <f t="shared" si="6"/>
+        <v>61.380774156924666</v>
       </c>
       <c r="I35" s="58">
-        <f t="shared" si="3"/>
-        <v>0</v>
+        <f t="shared" si="4"/>
+        <v>139.38550798134975</v>
       </c>
       <c r="J35" s="32">
         <f>'WTG Yield Wake'!I31*8760/100</f>
         <v>123.95399999999999</v>
       </c>
-      <c r="K35" s="116">
-        <f t="shared" si="4"/>
-        <v>0</v>
-      </c>
-    </row>
-    <row r="36" spans="1:13" ht="12.9" x14ac:dyDescent="0.35">
+      <c r="K35" s="107">
+        <f t="shared" si="5"/>
+        <v>17.277391256320225</v>
+      </c>
+    </row>
+    <row r="36" spans="1:13" ht="13.15" x14ac:dyDescent="0.4">
       <c r="B36" s="20">
         <v>18.5</v>
       </c>
@@ -6389,37 +6463,40 @@
         <f>'WTG Yield Wake'!D32</f>
         <v>20</v>
       </c>
-      <c r="D36" s="64"/>
+      <c r="D36" s="64">
+        <f t="shared" si="3"/>
+        <v>21.05263157894737</v>
+      </c>
       <c r="E36" s="62">
+        <f t="shared" si="7"/>
+        <v>6.3938306413463195</v>
+      </c>
+      <c r="F36" s="57">
         <f t="shared" si="6"/>
-        <v>0</v>
-      </c>
-      <c r="F36" s="57">
-        <f t="shared" si="5"/>
-        <v>0</v>
+        <v>25.575322565385278</v>
       </c>
       <c r="G36" s="57">
-        <f t="shared" si="5"/>
-        <v>0</v>
+        <f t="shared" si="6"/>
+        <v>46.035580617693491</v>
       </c>
       <c r="H36" s="57">
-        <f t="shared" si="5"/>
-        <v>0</v>
+        <f t="shared" si="6"/>
+        <v>61.380774156924666</v>
       </c>
       <c r="I36" s="58">
-        <f t="shared" si="3"/>
-        <v>0</v>
+        <f t="shared" si="4"/>
+        <v>139.38550798134975</v>
       </c>
       <c r="J36" s="32">
         <f>'WTG Yield Wake'!I32*8760/100</f>
         <v>100.38959999999999</v>
       </c>
-      <c r="K36" s="116">
-        <f t="shared" si="4"/>
-        <v>0</v>
-      </c>
-    </row>
-    <row r="37" spans="1:13" ht="12.9" x14ac:dyDescent="0.35">
+      <c r="K36" s="107">
+        <f t="shared" si="5"/>
+        <v>13.992855392044506</v>
+      </c>
+    </row>
+    <row r="37" spans="1:13" ht="13.15" x14ac:dyDescent="0.4">
       <c r="B37" s="20">
         <v>19.5</v>
       </c>
@@ -6427,37 +6504,40 @@
         <f>'WTG Yield Wake'!D33</f>
         <v>20</v>
       </c>
-      <c r="D37" s="64"/>
+      <c r="D37" s="64">
+        <f t="shared" si="3"/>
+        <v>21.05263157894737</v>
+      </c>
       <c r="E37" s="62">
-        <f t="shared" si="6"/>
-        <v>0</v>
+        <f t="shared" si="7"/>
+        <v>6.3938306413463195</v>
       </c>
       <c r="F37" s="57">
-        <f t="shared" si="6"/>
-        <v>0</v>
+        <f t="shared" si="7"/>
+        <v>25.575322565385278</v>
       </c>
       <c r="G37" s="57">
-        <f t="shared" si="6"/>
-        <v>0</v>
+        <f t="shared" si="7"/>
+        <v>46.035580617693491</v>
       </c>
       <c r="H37" s="57">
-        <f t="shared" si="6"/>
-        <v>0</v>
+        <f t="shared" si="7"/>
+        <v>61.380774156924666</v>
       </c>
       <c r="I37" s="58">
-        <f t="shared" si="3"/>
-        <v>0</v>
+        <f t="shared" si="4"/>
+        <v>139.38550798134975</v>
       </c>
       <c r="J37" s="32">
         <f>'WTG Yield Wake'!I33*8760/100</f>
         <v>75.686400000000006</v>
       </c>
-      <c r="K37" s="116">
-        <f t="shared" si="4"/>
-        <v>0</v>
-      </c>
-    </row>
-    <row r="38" spans="1:13" ht="12.9" x14ac:dyDescent="0.35">
+      <c r="K37" s="107">
+        <f t="shared" si="5"/>
+        <v>10.54958731127963</v>
+      </c>
+    </row>
+    <row r="38" spans="1:13" ht="13.15" x14ac:dyDescent="0.4">
       <c r="B38" s="20">
         <v>20.5</v>
       </c>
@@ -6465,37 +6545,40 @@
         <f>'WTG Yield Wake'!D34</f>
         <v>20</v>
       </c>
-      <c r="D38" s="64"/>
+      <c r="D38" s="64">
+        <f t="shared" si="3"/>
+        <v>21.05263157894737</v>
+      </c>
       <c r="E38" s="62">
-        <f t="shared" si="6"/>
-        <v>0</v>
+        <f t="shared" si="7"/>
+        <v>6.3938306413463195</v>
       </c>
       <c r="F38" s="57">
-        <f t="shared" si="6"/>
-        <v>0</v>
+        <f t="shared" si="7"/>
+        <v>25.575322565385278</v>
       </c>
       <c r="G38" s="57">
-        <f t="shared" si="6"/>
-        <v>0</v>
+        <f t="shared" si="7"/>
+        <v>46.035580617693491</v>
       </c>
       <c r="H38" s="57">
-        <f t="shared" si="6"/>
-        <v>0</v>
+        <f t="shared" si="7"/>
+        <v>61.380774156924666</v>
       </c>
       <c r="I38" s="58">
-        <f t="shared" si="3"/>
-        <v>0</v>
+        <f t="shared" si="4"/>
+        <v>139.38550798134975</v>
       </c>
       <c r="J38" s="32">
         <f>'WTG Yield Wake'!I34*8760/100</f>
         <v>53.611199999999997</v>
       </c>
-      <c r="K38" s="116">
-        <f t="shared" si="4"/>
-        <v>0</v>
-      </c>
-    </row>
-    <row r="39" spans="1:13" ht="12.9" x14ac:dyDescent="0.35">
+      <c r="K38" s="107">
+        <f t="shared" si="5"/>
+        <v>7.472624345489737</v>
+      </c>
+    </row>
+    <row r="39" spans="1:13" ht="13.15" x14ac:dyDescent="0.4">
       <c r="B39" s="20">
         <v>21.5</v>
       </c>
@@ -6503,37 +6586,40 @@
         <f>'WTG Yield Wake'!D35</f>
         <v>20</v>
       </c>
-      <c r="D39" s="64"/>
+      <c r="D39" s="64">
+        <f t="shared" si="3"/>
+        <v>21.05263157894737</v>
+      </c>
       <c r="E39" s="62">
-        <f t="shared" si="6"/>
-        <v>0</v>
+        <f t="shared" si="7"/>
+        <v>6.3938306413463195</v>
       </c>
       <c r="F39" s="57">
-        <f t="shared" si="6"/>
-        <v>0</v>
+        <f t="shared" si="7"/>
+        <v>25.575322565385278</v>
       </c>
       <c r="G39" s="57">
-        <f t="shared" si="6"/>
-        <v>0</v>
+        <f t="shared" si="7"/>
+        <v>46.035580617693491</v>
       </c>
       <c r="H39" s="57">
-        <f t="shared" si="6"/>
-        <v>0</v>
+        <f t="shared" si="7"/>
+        <v>61.380774156924666</v>
       </c>
       <c r="I39" s="58">
-        <f t="shared" si="3"/>
-        <v>0</v>
+        <f t="shared" si="4"/>
+        <v>139.38550798134975</v>
       </c>
       <c r="J39" s="32">
         <f>'WTG Yield Wake'!I35*8760/100</f>
         <v>38.106000000000002</v>
       </c>
-      <c r="K39" s="116">
-        <f t="shared" si="4"/>
-        <v>0</v>
-      </c>
-    </row>
-    <row r="40" spans="1:13" ht="12.9" x14ac:dyDescent="0.35">
+      <c r="K39" s="107">
+        <f t="shared" si="5"/>
+        <v>5.3114241671373135</v>
+      </c>
+    </row>
+    <row r="40" spans="1:13" ht="13.15" x14ac:dyDescent="0.4">
       <c r="B40" s="20">
         <v>22.5</v>
       </c>
@@ -6541,37 +6627,40 @@
         <f>'WTG Yield Wake'!D36</f>
         <v>20</v>
       </c>
-      <c r="D40" s="64"/>
+      <c r="D40" s="64">
+        <f t="shared" si="3"/>
+        <v>21.05263157894737</v>
+      </c>
       <c r="E40" s="62">
-        <f t="shared" si="6"/>
-        <v>0</v>
+        <f t="shared" si="7"/>
+        <v>6.3938306413463195</v>
       </c>
       <c r="F40" s="57">
-        <f t="shared" si="6"/>
-        <v>0</v>
+        <f t="shared" si="7"/>
+        <v>25.575322565385278</v>
       </c>
       <c r="G40" s="57">
-        <f t="shared" si="6"/>
-        <v>0</v>
+        <f t="shared" si="7"/>
+        <v>46.035580617693491</v>
       </c>
       <c r="H40" s="57">
-        <f t="shared" si="6"/>
-        <v>0</v>
+        <f t="shared" si="7"/>
+        <v>61.380774156924666</v>
       </c>
       <c r="I40" s="58">
-        <f t="shared" si="3"/>
-        <v>0</v>
+        <f t="shared" si="4"/>
+        <v>139.38550798134975</v>
       </c>
       <c r="J40" s="32">
         <f>'WTG Yield Wake'!I36*8760/100</f>
         <v>25.7544</v>
       </c>
-      <c r="K40" s="116">
-        <f t="shared" si="4"/>
-        <v>0</v>
-      </c>
-    </row>
-    <row r="41" spans="1:13" ht="12.9" x14ac:dyDescent="0.35">
+      <c r="K40" s="107">
+        <f t="shared" si="5"/>
+        <v>3.589790126754874</v>
+      </c>
+    </row>
+    <row r="41" spans="1:13" ht="13.15" x14ac:dyDescent="0.4">
       <c r="B41" s="20">
         <v>23.5</v>
       </c>
@@ -6579,37 +6668,40 @@
         <f>'WTG Yield Wake'!D37</f>
         <v>18.400000000000002</v>
       </c>
-      <c r="D41" s="64"/>
+      <c r="D41" s="64">
+        <f t="shared" si="3"/>
+        <v>19.368421052631582</v>
+      </c>
       <c r="E41" s="62">
-        <f t="shared" si="6"/>
-        <v>0</v>
+        <f t="shared" si="7"/>
+        <v>5.4117382548355275</v>
       </c>
       <c r="F41" s="57">
-        <f t="shared" si="6"/>
-        <v>0</v>
+        <f t="shared" si="7"/>
+        <v>21.64695301934211</v>
       </c>
       <c r="G41" s="57">
-        <f t="shared" si="6"/>
-        <v>0</v>
+        <f t="shared" si="7"/>
+        <v>38.964515434815787</v>
       </c>
       <c r="H41" s="57">
-        <f t="shared" si="6"/>
-        <v>0</v>
+        <f t="shared" si="7"/>
+        <v>51.952687246421064</v>
       </c>
       <c r="I41" s="58">
-        <f t="shared" si="3"/>
-        <v>0</v>
+        <f t="shared" si="4"/>
+        <v>117.97589395541449</v>
       </c>
       <c r="J41" s="32">
         <f>'WTG Yield Wake'!I37*8760/100</f>
         <v>15.855599999999999</v>
       </c>
-      <c r="K41" s="116">
-        <f t="shared" si="4"/>
-        <v>0</v>
-      </c>
-    </row>
-    <row r="42" spans="1:13" ht="12.9" x14ac:dyDescent="0.35">
+      <c r="K41" s="107">
+        <f t="shared" si="5"/>
+        <v>1.8705785841994698</v>
+      </c>
+    </row>
+    <row r="42" spans="1:13" ht="13.15" x14ac:dyDescent="0.4">
       <c r="B42" s="20">
         <v>24.5</v>
       </c>
@@ -6617,37 +6709,40 @@
         <f>'WTG Yield Wake'!D38</f>
         <v>15.200000000000001</v>
       </c>
-      <c r="D42" s="64"/>
+      <c r="D42" s="64">
+        <f t="shared" si="3"/>
+        <v>16.000000000000004</v>
+      </c>
       <c r="E42" s="62">
-        <f t="shared" si="6"/>
-        <v>0</v>
+        <f t="shared" si="7"/>
+        <v>3.6930765784416368</v>
       </c>
       <c r="F42" s="57">
-        <f t="shared" si="6"/>
-        <v>0</v>
+        <f t="shared" si="7"/>
+        <v>14.772306313766547</v>
       </c>
       <c r="G42" s="57">
-        <f t="shared" si="6"/>
-        <v>0</v>
+        <f t="shared" si="7"/>
+        <v>26.590151364779782</v>
       </c>
       <c r="H42" s="57">
-        <f t="shared" si="6"/>
-        <v>0</v>
+        <f t="shared" si="7"/>
+        <v>35.453535153039709</v>
       </c>
       <c r="I42" s="58">
-        <f t="shared" si="3"/>
-        <v>0</v>
+        <f t="shared" si="4"/>
+        <v>80.509069410027678</v>
       </c>
       <c r="J42" s="32">
         <f>'WTG Yield Wake'!I38*8760/100</f>
         <v>9.5484000000000009</v>
       </c>
-      <c r="K42" s="116">
-        <f t="shared" si="4"/>
-        <v>0</v>
-      </c>
-    </row>
-    <row r="43" spans="1:13" ht="12.9" x14ac:dyDescent="0.35">
+      <c r="K42" s="107">
+        <f t="shared" si="5"/>
+        <v>0.76873279835470842</v>
+      </c>
+    </row>
+    <row r="43" spans="1:13" ht="13.15" x14ac:dyDescent="0.4">
       <c r="B43" s="20">
         <v>25.5</v>
       </c>
@@ -6655,37 +6750,40 @@
         <f>'WTG Yield Wake'!D39</f>
         <v>12</v>
       </c>
-      <c r="D43" s="64"/>
+      <c r="D43" s="64">
+        <f t="shared" si="3"/>
+        <v>12.631578947368421</v>
+      </c>
       <c r="E43" s="62">
-        <f t="shared" si="6"/>
-        <v>0</v>
+        <f t="shared" si="7"/>
+        <v>2.3017790308846746</v>
       </c>
       <c r="F43" s="57">
-        <f t="shared" si="6"/>
-        <v>0</v>
+        <f t="shared" si="7"/>
+        <v>9.2071161235386985</v>
       </c>
       <c r="G43" s="57">
-        <f t="shared" si="6"/>
-        <v>0</v>
+        <f t="shared" si="7"/>
+        <v>16.572809022369661</v>
       </c>
       <c r="H43" s="57">
-        <f t="shared" si="6"/>
-        <v>0</v>
+        <f t="shared" si="7"/>
+        <v>22.097078696492879</v>
       </c>
       <c r="I43" s="58">
-        <f t="shared" si="3"/>
-        <v>0</v>
+        <f t="shared" si="4"/>
+        <v>50.178782873285911</v>
       </c>
       <c r="J43" s="32">
         <f>'WTG Yield Wake'!I39*8760/100</f>
         <v>6.2195999999999989</v>
       </c>
-      <c r="K43" s="116">
-        <f t="shared" si="4"/>
-        <v>0</v>
-      </c>
-    </row>
-    <row r="44" spans="1:13" ht="12.9" x14ac:dyDescent="0.35">
+      <c r="K43" s="107">
+        <f t="shared" si="5"/>
+        <v>0.31209195795868905</v>
+      </c>
+    </row>
+    <row r="44" spans="1:13" ht="13.15" x14ac:dyDescent="0.4">
       <c r="B44" s="20">
         <v>26.5</v>
       </c>
@@ -6693,37 +6791,40 @@
         <f>'WTG Yield Wake'!D40</f>
         <v>8.7999999999999989</v>
       </c>
-      <c r="D44" s="64"/>
+      <c r="D44" s="64">
+        <f t="shared" si="3"/>
+        <v>9.2631578947368407</v>
+      </c>
       <c r="E44" s="62">
-        <f t="shared" si="6"/>
-        <v>0</v>
+        <f t="shared" si="7"/>
+        <v>1.2378456121646471</v>
       </c>
       <c r="F44" s="57">
-        <f t="shared" si="6"/>
-        <v>0</v>
+        <f t="shared" si="7"/>
+        <v>4.9513824486585882</v>
       </c>
       <c r="G44" s="57">
-        <f t="shared" si="6"/>
-        <v>0</v>
+        <f t="shared" si="7"/>
+        <v>8.9124884075854585</v>
       </c>
       <c r="H44" s="57">
-        <f t="shared" si="6"/>
-        <v>0</v>
+        <f t="shared" si="7"/>
+        <v>11.883317876780612</v>
       </c>
       <c r="I44" s="58">
-        <f t="shared" si="3"/>
-        <v>0</v>
+        <f t="shared" si="4"/>
+        <v>26.985034345189305</v>
       </c>
       <c r="J44" s="32">
         <f>'WTG Yield Wake'!I40*8760/100</f>
         <v>3.4163999999999999</v>
       </c>
-      <c r="K44" s="116">
-        <f t="shared" si="4"/>
-        <v>0</v>
-      </c>
-    </row>
-    <row r="45" spans="1:13" ht="12.9" x14ac:dyDescent="0.35">
+      <c r="K44" s="107">
+        <f t="shared" si="5"/>
+        <v>9.2191671336904729E-2</v>
+      </c>
+    </row>
+    <row r="45" spans="1:13" ht="13.15" x14ac:dyDescent="0.4">
       <c r="B45" s="20">
         <v>27.5</v>
       </c>
@@ -6731,37 +6832,40 @@
         <f>'WTG Yield Wake'!D41</f>
         <v>5.6</v>
       </c>
-      <c r="D45" s="64"/>
+      <c r="D45" s="64">
+        <f t="shared" si="3"/>
+        <v>5.8947368421052628</v>
+      </c>
       <c r="E45" s="62">
-        <f t="shared" si="6"/>
-        <v>0</v>
+        <f t="shared" si="7"/>
+        <v>0.50127632228155139</v>
       </c>
       <c r="F45" s="57">
-        <f t="shared" si="6"/>
-        <v>0</v>
+        <f t="shared" si="7"/>
+        <v>2.0051052891262056</v>
       </c>
       <c r="G45" s="57">
-        <f t="shared" si="6"/>
-        <v>0</v>
+        <f t="shared" si="7"/>
+        <v>3.60918952042717</v>
       </c>
       <c r="H45" s="57">
-        <f t="shared" si="6"/>
-        <v>0</v>
+        <f t="shared" si="7"/>
+        <v>4.8122526939028933</v>
       </c>
       <c r="I45" s="58">
-        <f t="shared" si="3"/>
-        <v>0</v>
+        <f t="shared" si="4"/>
+        <v>10.927823825737821</v>
       </c>
       <c r="J45" s="32">
         <f>'WTG Yield Wake'!I41*8760/100</f>
         <v>2.3652000000000002</v>
       </c>
-      <c r="K45" s="116">
-        <f t="shared" si="4"/>
-        <v>0</v>
-      </c>
-    </row>
-    <row r="46" spans="1:13" ht="13.3" thickBot="1" x14ac:dyDescent="0.4">
+      <c r="K45" s="107">
+        <f t="shared" si="5"/>
+        <v>2.5846488912635097E-2</v>
+      </c>
+    </row>
+    <row r="46" spans="1:13" ht="13.5" thickBot="1" x14ac:dyDescent="0.45">
       <c r="B46" s="25">
         <v>28.5</v>
       </c>
@@ -6769,36 +6873,39 @@
         <f>'WTG Yield Wake'!D42</f>
         <v>0</v>
       </c>
-      <c r="D46" s="65"/>
-      <c r="E46" s="75">
-        <f t="shared" si="6"/>
+      <c r="D46" s="65">
+        <f>C46/0.95</f>
         <v>0</v>
       </c>
-      <c r="F46" s="76">
-        <f t="shared" si="6"/>
+      <c r="E46" s="73">
+        <f t="shared" si="7"/>
         <v>0</v>
       </c>
-      <c r="G46" s="76">
-        <f t="shared" si="6"/>
+      <c r="F46" s="74">
+        <f t="shared" si="7"/>
         <v>0</v>
       </c>
-      <c r="H46" s="76">
-        <f t="shared" si="6"/>
+      <c r="G46" s="74">
+        <f t="shared" si="7"/>
         <v>0</v>
       </c>
+      <c r="H46" s="74">
+        <f t="shared" si="7"/>
+        <v>0</v>
+      </c>
       <c r="I46" s="53">
-        <f t="shared" si="3"/>
+        <f t="shared" si="4"/>
         <v>0</v>
       </c>
       <c r="J46" s="37">
         <v>1</v>
       </c>
-      <c r="K46" s="117">
-        <f t="shared" si="4"/>
+      <c r="K46" s="108">
+        <f t="shared" si="5"/>
         <v>0</v>
       </c>
     </row>
-    <row r="47" spans="1:13" ht="12.9" x14ac:dyDescent="0.35">
+    <row r="47" spans="1:13" ht="13.15" x14ac:dyDescent="0.4">
       <c r="A47" s="9"/>
       <c r="B47" s="9"/>
       <c r="C47" s="9"/>
@@ -6808,16 +6915,16 @@
       <c r="G47" s="9"/>
       <c r="H47" s="9"/>
       <c r="I47" s="9"/>
-      <c r="J47" s="87">
+      <c r="J47" s="79">
         <f>SUM(J18:J46)</f>
         <v>8759.3080000000009</v>
       </c>
-      <c r="K47" s="84"/>
+      <c r="K47" s="76"/>
       <c r="L47" s="3" t="s">
         <v>55</v>
       </c>
     </row>
-    <row r="48" spans="1:13" ht="13.3" thickBot="1" x14ac:dyDescent="0.4">
+    <row r="48" spans="1:13" ht="13.5" thickBot="1" x14ac:dyDescent="0.45">
       <c r="A48" s="9"/>
       <c r="B48" s="3" t="s">
         <v>60</v>
@@ -6829,17 +6936,17 @@
       <c r="G48" s="3"/>
       <c r="H48" s="3"/>
       <c r="I48" s="3"/>
-      <c r="J48" s="85"/>
-      <c r="K48" s="86">
+      <c r="J48" s="77"/>
+      <c r="K48" s="78">
         <f>SUM(K18:K47)</f>
-        <v>0</v>
+        <v>559.56786886587042</v>
       </c>
       <c r="L48" s="3" t="s">
         <v>28</v>
       </c>
       <c r="M48" s="1"/>
     </row>
-    <row r="49" spans="1:13" ht="12.9" x14ac:dyDescent="0.35">
+    <row r="49" spans="1:13" ht="13.15" x14ac:dyDescent="0.4">
       <c r="A49" s="9"/>
       <c r="B49" s="3" t="s">
         <v>61</v>
@@ -6851,14 +6958,17 @@
       <c r="G49" s="3"/>
       <c r="H49" s="3"/>
       <c r="I49" s="3"/>
-      <c r="J49" s="85"/>
-      <c r="K49" s="92"/>
+      <c r="J49" s="77"/>
+      <c r="K49" s="84">
+        <f>'WTG Yield Wake'!J43*4</f>
+        <v>395260.31275559997</v>
+      </c>
       <c r="L49" s="3" t="s">
         <v>28</v>
       </c>
       <c r="M49" s="1"/>
     </row>
-    <row r="50" spans="1:13" ht="13.3" thickBot="1" x14ac:dyDescent="0.4">
+    <row r="50" spans="1:13" ht="13.5" thickBot="1" x14ac:dyDescent="0.45">
       <c r="A50" s="9"/>
       <c r="B50" s="3" t="s">
         <v>64</v>
@@ -6870,13 +6980,16 @@
       <c r="G50" s="3"/>
       <c r="H50" s="3"/>
       <c r="I50" s="3"/>
-      <c r="J50" s="85"/>
-      <c r="K50" s="93"/>
+      <c r="J50" s="77"/>
+      <c r="K50" s="85">
+        <f>(K48/K49)</f>
+        <v>1.4156945456142119E-3</v>
+      </c>
       <c r="L50" s="3" t="s">
         <v>51</v>
       </c>
     </row>
-    <row r="51" spans="1:13" x14ac:dyDescent="0.3">
+    <row r="51" spans="1:13" x14ac:dyDescent="0.35">
       <c r="J51" s="33"/>
     </row>
   </sheetData>

</xml_diff>